<commit_message>
updates for test problems
</commit_message>
<xml_diff>
--- a/src/data/3_comp_test.xlsx
+++ b/src/data/3_comp_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\sns_modeling\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\Braskem Project\test problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656246D1-A7D9-40E2-B01A-07E86872A288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63C212C-4600-4BA8-B9AA-3A452DF82797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>